<commit_message>
Clássica, Frequentista e Axiomática
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb5670dbed6d0692/Documentos/Python Scripts/prevendo futuro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="11_F25DC773A252ABDACC1048DDD1585AB65ADE58FA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{602F7701-D70B-4E82-9165-5B982E2A39CE}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="11_F25DC773A252ABDACC1048DDD1585AB65ADE58FA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B8777B2-7434-4622-9723-E13D1C9126AF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId5"/>
+    <pivotCache cacheId="3" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="68">
   <si>
     <t>Idade (anos)</t>
   </si>
@@ -254,6 +254,57 @@
   </si>
   <si>
     <t>Probabilidade de ter um salário acima do valor P5</t>
+  </si>
+  <si>
+    <t>Rótulos de Coluna</t>
+  </si>
+  <si>
+    <t>Total de compras:</t>
+  </si>
+  <si>
+    <t>Total registros:</t>
+  </si>
+  <si>
+    <t>% de Compra</t>
+  </si>
+  <si>
+    <t>Calcular a Probabilidade de Compra</t>
+  </si>
+  <si>
+    <t>% SIM</t>
+  </si>
+  <si>
+    <t>Calcular a Probabilidade de Compra com Base na Idade</t>
+  </si>
+  <si>
+    <t>22-28</t>
+  </si>
+  <si>
+    <t>29-35</t>
+  </si>
+  <si>
+    <t>36-42</t>
+  </si>
+  <si>
+    <t>Construir o Modelo Probabilístico</t>
+  </si>
+  <si>
+    <t>P(A e B) = P(A|B) * P(B)</t>
+  </si>
+  <si>
+    <t>Calcular a Probabilidade Condicional - GENERO</t>
+  </si>
+  <si>
+    <t>% masc</t>
+  </si>
+  <si>
+    <t>% fem</t>
+  </si>
+  <si>
+    <t>Probabilidade de compra masculina</t>
+  </si>
+  <si>
+    <t>Probabilidade de compra feminina</t>
   </si>
 </sst>
 </file>
@@ -319,7 +370,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,8 +389,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -448,12 +505,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -462,7 +528,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -471,15 +537,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -505,34 +567,169 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="29">
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -606,44 +803,17 @@
       </border>
     </dxf>
     <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -681,69 +851,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -786,6 +894,16 @@
         <n v="41"/>
         <n v="42"/>
       </sharedItems>
+      <fieldGroup base="0">
+        <rangePr startNum="22" endNum="42" groupInterval="7"/>
+        <groupItems count="5">
+          <s v="&lt;22"/>
+          <s v="22-28"/>
+          <s v="29-35"/>
+          <s v="36-42"/>
+          <s v="&gt;43"/>
+        </groupItems>
+      </fieldGroup>
     </cacheField>
     <cacheField name="Salário (R$)" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2500" maxValue="6500"/>
@@ -997,30 +1115,16 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{291EB4B1-8DC7-4CB6-94B5-2CB65A5822A6}" name="Tabela dinâmica2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total_x000a_Geral" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Idade" colHeaderCaption="Comprou">
-  <location ref="A2:D23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{291EB4B1-8DC7-4CB6-94B5-2CB65A5822A6}" name="Tabela dinâmica2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total_x000a_Geral" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Idade" colHeaderCaption="Comprou">
+  <location ref="A2:D7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
-      <items count="20">
+      <items count="6">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1037,10 +1141,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="20">
-    <i>
-      <x/>
-    </i>
+  <rowItems count="4">
     <i>
       <x v="1"/>
     </i>
@@ -1049,51 +1150,6 @@
     </i>
     <i>
       <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
     </i>
     <i t="grand">
       <x/>
@@ -1117,7 +1173,7 @@
     <dataField name="Contagem de Comprou (Sim/Não)" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="7">
-    <format dxfId="8">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -1126,7 +1182,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -1135,7 +1191,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="19">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -1143,20 +1199,20 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="18">
       <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -1173,10 +1229,95 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{165666D8-D590-4812-95B5-3AB53EC9D1FE}" name="Tabela dinâmica6" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A2:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9E035A05-ED20-4017-9822-A64CA4F825E8}" name="Tabela dinâmica2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B22:E27" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Contagem de Comprou (Sim/Não)" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B6289D42-3DE4-4C3E-BF82-C11FA4AEB5A1}" name="Tabela dinâmica1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B10:E14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="3">
@@ -1185,7 +1326,13 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
   </pivotFields>
   <rowFields count="1">
     <field x="2"/>
@@ -1201,8 +1348,19 @@
       <x/>
     </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
   </colItems>
   <dataFields count="1">
     <dataField name="Contagem de Comprou (Sim/Não)" fld="3" subtotal="count" baseField="0" baseItem="0"/>
@@ -1220,16 +1378,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BA061FA-C831-4293-A7E5-7C018712B2AA}" name="Tabela1" displayName="Tabela1" ref="A1:D31" totalsRowShown="0" headerRowDxfId="9" dataDxfId="10" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BA061FA-C831-4293-A7E5-7C018712B2AA}" name="Tabela1" displayName="Tabela1" ref="A1:D31" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
   <autoFilter ref="A1:D31" xr:uid="{9BA061FA-C831-4293-A7E5-7C018712B2AA}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D31">
     <sortCondition ref="A1:A31"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{91C97254-4D9E-4627-AA3A-941152FF9BB4}" name="Idade (anos)" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{5CEBC119-22C0-46B2-B9E6-6679A3E33F56}" name="Salário (R$)" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{EA5C05E1-69CD-43E2-85CD-ABFC4209B848}" name="Gênero" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{7333478C-6724-4429-B2FF-19B89F9F26C7}" name="Comprou (Sim/Não)" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{91C97254-4D9E-4627-AA3A-941152FF9BB4}" name="Idade (anos)" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{5CEBC119-22C0-46B2-B9E6-6679A3E33F56}" name="Salário (R$)" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{EA5C05E1-69CD-43E2-85CD-ABFC4209B848}" name="Gênero" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{7333478C-6724-4429-B2FF-19B89F9F26C7}" name="Comprou (Sim/Não)" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1530,10 +1688,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19">
+      <c r="A2" s="17">
         <v>22</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="19">
         <v>2500</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1544,10 +1702,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19">
+      <c r="A3" s="17">
         <v>25</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="19">
         <v>3000</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1558,10 +1716,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19">
+      <c r="A4" s="17">
         <v>25</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="19">
         <v>2900</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1575,10 +1733,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19">
+      <c r="A5" s="17">
         <v>26</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="19">
         <v>3000</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1592,10 +1750,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19">
+      <c r="A6" s="17">
         <v>27</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="19">
         <v>3500</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1609,10 +1767,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19">
+      <c r="A7" s="17">
         <v>27</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="19">
         <v>3100</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1626,10 +1784,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19">
+      <c r="A8" s="17">
         <v>28</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="19">
         <v>4500</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1640,10 +1798,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19">
+      <c r="A9" s="17">
         <v>28</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="19">
         <v>3400</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1654,10 +1812,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19">
+      <c r="A10" s="17">
         <v>29</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="19">
         <v>3700</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1668,10 +1826,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19">
+      <c r="A11" s="17">
         <v>29</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="19">
         <v>3600</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1682,10 +1840,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19">
+      <c r="A12" s="17">
         <v>30</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="19">
         <v>4000</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1696,10 +1854,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19">
+      <c r="A13" s="17">
         <v>30</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="19">
         <v>4300</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1710,10 +1868,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19">
+      <c r="A14" s="17">
         <v>31</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="19">
         <v>4200</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1724,10 +1882,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19">
+      <c r="A15" s="17">
         <v>31</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="19">
         <v>4500</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1738,10 +1896,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19">
+      <c r="A16" s="17">
         <v>32</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="19">
         <v>4400</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1752,10 +1910,10 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19">
+      <c r="A17" s="17">
         <v>33</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="19">
         <v>4900</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1766,10 +1924,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19">
+      <c r="A18" s="17">
         <v>33</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="19">
         <v>4800</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1780,10 +1938,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19">
+      <c r="A19" s="17">
         <v>34</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="19">
         <v>4600</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1794,10 +1952,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19">
+      <c r="A20" s="17">
         <v>35</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="19">
         <v>5500</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1808,10 +1966,10 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="19">
+      <c r="A21" s="17">
         <v>35</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="19">
         <v>6000</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1822,10 +1980,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19">
+      <c r="A22" s="17">
         <v>35</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="19">
         <v>5300</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1836,10 +1994,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="19">
+      <c r="A23" s="17">
         <v>36</v>
       </c>
-      <c r="B23" s="21">
+      <c r="B23" s="19">
         <v>5200</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1850,10 +2008,10 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19">
+      <c r="A24" s="17">
         <v>36</v>
       </c>
-      <c r="B24" s="21">
+      <c r="B24" s="19">
         <v>5400</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1864,10 +2022,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="19">
+      <c r="A25" s="17">
         <v>37</v>
       </c>
-      <c r="B25" s="21">
+      <c r="B25" s="19">
         <v>5500</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1878,10 +2036,10 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="19">
+      <c r="A26" s="17">
         <v>38</v>
       </c>
-      <c r="B26" s="21">
+      <c r="B26" s="19">
         <v>5700</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1892,10 +2050,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="19">
+      <c r="A27" s="17">
         <v>39</v>
       </c>
-      <c r="B27" s="21">
+      <c r="B27" s="19">
         <v>5900</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1906,10 +2064,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="19">
+      <c r="A28" s="17">
         <v>40</v>
       </c>
-      <c r="B28" s="21">
+      <c r="B28" s="19">
         <v>5800</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1920,10 +2078,10 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="19">
+      <c r="A29" s="17">
         <v>40</v>
       </c>
-      <c r="B29" s="21">
+      <c r="B29" s="19">
         <v>6000</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1934,10 +2092,10 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19">
+      <c r="A30" s="17">
         <v>41</v>
       </c>
-      <c r="B30" s="21">
+      <c r="B30" s="19">
         <v>6200</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1948,10 +2106,10 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="20">
+      <c r="A31" s="18">
         <v>42</v>
       </c>
-      <c r="B31" s="22">
+      <c r="B31" s="20">
         <v>6500</v>
       </c>
       <c r="C31" s="5" t="s">
@@ -1974,7 +2132,7 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A2:I23"/>
+  <dimension ref="A2:I22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
@@ -1985,34 +2143,34 @@
     <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="11" t="s">
         <v>18</v>
       </c>
       <c r="I3" t="s">
@@ -2020,329 +2178,165 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>22</v>
-      </c>
-      <c r="B4" s="11">
+      <c r="A4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="30">
+        <v>7</v>
+      </c>
+      <c r="C4" s="30">
         <v>1</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11">
+      <c r="D4" s="30">
+        <v>8</v>
+      </c>
+      <c r="E4" s="12" t="e">
+        <f>B4/$D$23</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="30">
+        <v>6</v>
+      </c>
+      <c r="C5" s="30">
+        <v>7</v>
+      </c>
+      <c r="D5" s="30">
+        <v>13</v>
+      </c>
+      <c r="E5" s="13" t="e">
+        <f t="shared" ref="E5:E22" si="0">B5/$D$23</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="30">
+        <v>8</v>
+      </c>
+      <c r="C6" s="30">
         <v>1</v>
       </c>
-      <c r="E4" s="14">
-        <f>B4/$D$23</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>25</v>
-      </c>
-      <c r="B5" s="11">
-        <v>2</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11">
-        <v>2</v>
-      </c>
-      <c r="E5" s="15">
-        <f t="shared" ref="E5:E22" si="0">B5/$D$23</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
-        <v>26</v>
-      </c>
-      <c r="B6" s="11">
-        <v>1</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11">
-        <v>1</v>
-      </c>
-      <c r="E6" s="15">
+      <c r="D6" s="30">
+        <v>9</v>
+      </c>
+      <c r="E6" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>3.3333333333333333E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>27</v>
-      </c>
-      <c r="B7" s="11">
-        <v>2</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11">
-        <v>2</v>
-      </c>
-      <c r="E7" s="15">
+      <c r="A7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="28">
+        <v>21</v>
+      </c>
+      <c r="C7" s="28">
+        <v>9</v>
+      </c>
+      <c r="D7" s="28">
+        <v>30</v>
+      </c>
+      <c r="E7" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>6.6666666666666666E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>28</v>
-      </c>
-      <c r="B8" s="11">
-        <v>1</v>
-      </c>
-      <c r="C8" s="11">
-        <v>1</v>
-      </c>
-      <c r="D8" s="11">
-        <v>2</v>
-      </c>
-      <c r="E8" s="15">
+      <c r="E8" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>3.3333333333333333E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>29</v>
-      </c>
-      <c r="B9" s="11">
-        <v>2</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11">
-        <v>2</v>
-      </c>
-      <c r="E9" s="15">
+      <c r="E9" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>6.6666666666666666E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>30</v>
-      </c>
-      <c r="B10" s="11">
-        <v>1</v>
-      </c>
-      <c r="C10" s="11">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11">
-        <v>2</v>
-      </c>
-      <c r="E10" s="15">
+      <c r="E10" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>3.3333333333333333E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>31</v>
-      </c>
-      <c r="B11" s="11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="11">
-        <v>2</v>
-      </c>
-      <c r="E11" s="15">
+      <c r="E11" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>3.3333333333333333E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>32</v>
-      </c>
-      <c r="B12" s="11">
-        <v>1</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11">
-        <v>1</v>
-      </c>
-      <c r="E12" s="15">
+      <c r="E12" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>3.3333333333333333E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
-        <v>33</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11">
-        <v>2</v>
-      </c>
-      <c r="D13" s="11">
-        <v>2</v>
-      </c>
-      <c r="E13" s="15">
+      <c r="E13" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>34</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11">
-        <v>1</v>
-      </c>
-      <c r="D14" s="11">
-        <v>1</v>
-      </c>
-      <c r="E14" s="15">
+      <c r="E14" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
-        <v>35</v>
-      </c>
-      <c r="B15" s="11">
-        <v>1</v>
-      </c>
-      <c r="C15" s="11">
-        <v>2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>3</v>
-      </c>
-      <c r="E15" s="15">
+      <c r="E15" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>3.3333333333333333E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <v>36</v>
-      </c>
-      <c r="B16" s="11">
-        <v>2</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11">
-        <v>2</v>
-      </c>
-      <c r="E16" s="15">
+      <c r="E16" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>37</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11">
-        <v>1</v>
-      </c>
-      <c r="D17" s="11">
-        <v>1</v>
-      </c>
-      <c r="E17" s="15">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
-        <v>38</v>
-      </c>
-      <c r="B18" s="11">
-        <v>1</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11">
-        <v>1</v>
-      </c>
-      <c r="E18" s="15">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
-        <v>39</v>
-      </c>
-      <c r="B19" s="11">
-        <v>1</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11">
-        <v>1</v>
-      </c>
-      <c r="E19" s="15">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
-        <v>40</v>
-      </c>
-      <c r="B20" s="11">
-        <v>2</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11">
-        <v>2</v>
-      </c>
-      <c r="E20" s="15">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>41</v>
-      </c>
-      <c r="B21" s="11">
-        <v>1</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11">
-        <v>1</v>
-      </c>
-      <c r="E21" s="16">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="14" t="e">
         <f t="shared" si="0"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
-        <v>42</v>
-      </c>
-      <c r="B22" s="11">
-        <v>1</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11">
-        <v>1</v>
-      </c>
-      <c r="E22" s="12">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="7">
-        <v>21</v>
-      </c>
-      <c r="C23" s="7">
-        <v>9</v>
-      </c>
-      <c r="D23" s="7">
-        <v>30</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -2407,16 +2401,16 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="26"/>
+      <c r="B3" s="23"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4">
         <v>0.96582433199541773</v>
       </c>
       <c r="O4" t="s">
@@ -2427,10 +2421,10 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="24">
         <v>0.93281664027439493</v>
       </c>
       <c r="O5" t="s">
@@ -2442,18 +2436,18 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6">
         <v>0.93041723456990899</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7">
         <v>299.84151137756947</v>
       </c>
       <c r="O7" t="s">
@@ -2461,10 +2455,10 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="21">
         <v>30</v>
       </c>
       <c r="O8">
@@ -2478,20 +2472,20 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="22" t="s">
         <v>36</v>
       </c>
       <c r="O11" t="s">
@@ -2499,142 +2493,140 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12">
         <v>34952328.57220149</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12">
         <v>34952328.57220149</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12">
         <v>388.76986852636583</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12">
         <v>5.8913287510754522E-18</v>
       </c>
-      <c r="O12" s="12">
+      <c r="O12" s="10">
         <f xml:space="preserve"> 1 - O8</f>
         <v>0.99997368205388915</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13">
         <v>28</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13">
         <v>2517338.0944651836</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13">
         <v>89904.931945185133</v>
       </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="21">
         <v>29</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="21">
         <v>37469666.666666672</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25" t="s">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="I16" s="25" t="s">
+      <c r="I16" s="22" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17">
         <v>-2100.3408537575087</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17">
         <v>344.03557618856081</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17">
         <v>-6.1050106417085859</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17">
         <v>1.3802820361046674E-6</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17">
         <v>-2805.0657850537987</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17">
         <v>-1395.6159224612188</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17">
         <v>-2805.0657850537987</v>
       </c>
-      <c r="I17" s="23">
+      <c r="I17">
         <v>-1395.6159224612188</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="21">
         <v>206.27333225125795</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C18" s="21">
         <v>10.461568079662943</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="21">
         <v>19.717247995761625</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="21">
         <v>5.8913287510754938E-18</v>
       </c>
-      <c r="F18" s="24">
+      <c r="F18" s="21">
         <v>184.84378148249922</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="21">
         <v>227.70288302001669</v>
       </c>
-      <c r="H18" s="24">
+      <c r="H18" s="21">
         <v>184.84378148249922</v>
       </c>
-      <c r="I18" s="24">
+      <c r="I18" s="21">
         <v>227.70288302001669</v>
       </c>
     </row>
@@ -2648,144 +2640,311 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="29">
+        <f>D13/$E$14</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4">
+        <f>COUNTIF(Tabela1[Comprou (Sim/Não)],"Sim")</f>
+        <v>21</v>
+      </c>
+      <c r="E4" s="26"/>
+      <c r="H4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="29">
+        <f>D12/$E$14</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5">
+        <f>COUNTA(Tabela1[Comprou (Sim/Não)])</f>
+        <v>30</v>
+      </c>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="29">
+        <f>C4/C5</f>
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="28">
+        <v>3</v>
+      </c>
+      <c r="D12" s="28">
+        <v>12</v>
+      </c>
+      <c r="E12" s="28">
+        <v>15</v>
+      </c>
+      <c r="F12" s="10">
+        <f>D12/E12</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="28">
+        <v>6</v>
+      </c>
+      <c r="D13" s="28">
+        <v>9</v>
+      </c>
+      <c r="E13" s="28">
+        <v>15</v>
+      </c>
+      <c r="F13" s="10">
+        <f>D13/E13</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="28">
+        <v>9</v>
+      </c>
+      <c r="D14" s="28">
+        <v>21</v>
+      </c>
+      <c r="E14" s="28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="26"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="C22" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="28">
+        <v>1</v>
+      </c>
+      <c r="D24" s="28">
+        <v>7</v>
+      </c>
+      <c r="E24" s="28">
+        <v>8</v>
+      </c>
+      <c r="F24" s="10">
+        <f>D24/E24</f>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="28">
+        <v>7</v>
+      </c>
+      <c r="D25" s="28">
         <v>6</v>
       </c>
-      <c r="B3" s="7">
-        <v>15</v>
-      </c>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="7">
-        <v>15</v>
-      </c>
-      <c r="E4" s="32"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="E25" s="28">
         <v>13</v>
       </c>
-      <c r="B5" s="7">
+      <c r="F25" s="10">
+        <f t="shared" ref="F25:F26" si="0">D25/E25</f>
+        <v>0.46153846153846156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="28">
+        <v>1</v>
+      </c>
+      <c r="D26" s="28">
+        <v>8</v>
+      </c>
+      <c r="E26" s="28">
+        <v>9</v>
+      </c>
+      <c r="F26" s="10">
+        <f t="shared" si="0"/>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="28">
+        <v>9</v>
+      </c>
+      <c r="D27" s="28">
+        <v>21</v>
+      </c>
+      <c r="E27" s="28">
         <v>30</v>
       </c>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="32"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="12"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="12"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="12"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E27" s="12"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="31"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="31"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
+      <c r="B32" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="25"/>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G34" s="31">
+        <f xml:space="preserve"> (F12/F13) *I4</f>
+        <v>0.53333333333333344</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="31">
+        <f xml:space="preserve"> (F13/F12) *I4</f>
+        <v>0.3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>